<commit_message>
add scripts for last script on test 2
</commit_message>
<xml_diff>
--- a/2018_2019/Tests/Test 2 solutions/IEP scores 20182019 test 2.xlsx
+++ b/2018_2019/Tests/Test 2 solutions/IEP scores 20182019 test 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="11640" windowHeight="7005"/>
+    <workbookView xWindow="14880" yWindow="0" windowWidth="11640" windowHeight="7005"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00000000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -795,7 +795,7 @@
     <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1106,7 +1106,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
+      <selection pane="bottomLeft" activeCell="AG22" sqref="AG22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3585,39 +3585,101 @@
       <c r="G22" s="28"/>
       <c r="H22" s="36">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32"/>
-      <c r="AA22" s="32"/>
-      <c r="AB22" s="32"/>
-      <c r="AC22" s="32"/>
-      <c r="AD22" s="32"/>
-      <c r="AE22" s="32"/>
-      <c r="AF22" s="32"/>
-      <c r="AG22" s="33"/>
-      <c r="AH22" s="33"/>
-      <c r="AI22" s="31"/>
-      <c r="AJ22" s="31"/>
-      <c r="AK22" s="31"/>
-      <c r="AL22" s="31"/>
-      <c r="AM22" s="31"/>
+        <v>11.538461538461537</v>
+      </c>
+      <c r="I22" s="30">
+        <v>1</v>
+      </c>
+      <c r="J22" s="30">
+        <v>1</v>
+      </c>
+      <c r="K22" s="30">
+        <v>1</v>
+      </c>
+      <c r="L22" s="30">
+        <v>1</v>
+      </c>
+      <c r="M22" s="30">
+        <v>1</v>
+      </c>
+      <c r="N22" s="30">
+        <v>1</v>
+      </c>
+      <c r="O22" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="P22" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="Q22" s="30">
+        <v>1</v>
+      </c>
+      <c r="R22" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="S22" s="30">
+        <v>0</v>
+      </c>
+      <c r="T22" s="30">
+        <v>1</v>
+      </c>
+      <c r="U22" s="30">
+        <v>1</v>
+      </c>
+      <c r="V22" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="W22" s="31">
+        <v>0</v>
+      </c>
+      <c r="X22" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="Y22" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="32">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="AC22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="32">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="33">
+        <v>1</v>
+      </c>
+      <c r="AH22" s="33">
+        <v>1</v>
+      </c>
+      <c r="AI22" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="31">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">

</xml_diff>